<commit_message>
impressão de dados da planilha no python
</commit_message>
<xml_diff>
--- a/Planilha de Compras.xlsx
+++ b/Planilha de Compras.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,66 +443,83 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Banana</t>
+          <t>Frutas</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>Quantidade</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>R$3,90</t>
+          <t>Preço</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Fruta 2</t>
+          <t>Banana</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R$15,90</t>
+          <t>R$3,90</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Fruta 3</t>
+          <t>Fruta 2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>R$30,90</t>
+          <t>R$15,90</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Fruta 3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>R$30,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>Fruta 4</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>R$50,50</t>
         </is>

</xml_diff>